<commit_message>
made a few more variable volatile
</commit_message>
<xml_diff>
--- a/sfw/U701_firmware/Interrupt_Priority_List.xlsx
+++ b/sfw/U701_firmware/Interrupt_Priority_List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23378465-E42C-4F29-8183-C51653174BF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DB3561-5E83-48F2-8328-D25FBD864AEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3540" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Priority</t>
   </si>
@@ -46,15 +46,9 @@
     <t>Prefetch_Module_SEC_Event</t>
   </si>
   <si>
-    <t>SPI3_Fault</t>
-  </si>
-  <si>
     <t>UART3_Fault</t>
   </si>
   <si>
-    <t>SPI flash error</t>
-  </si>
-  <si>
     <t>heartbeat timer</t>
   </si>
   <si>
@@ -71,6 +65,54 @@
   </si>
   <si>
     <t>ADC Data 44</t>
+  </si>
+  <si>
+    <t>Context Savings</t>
+  </si>
+  <si>
+    <t>SRS</t>
+  </si>
+  <si>
+    <t>DMA_Channel_1</t>
+  </si>
+  <si>
+    <t>Handles USB UART RX DMA IRQ's</t>
+  </si>
+  <si>
+    <t>RTCC</t>
+  </si>
+  <si>
+    <t>RTCC timekeeping ISR</t>
+  </si>
+  <si>
+    <t>ADC Data 10</t>
+  </si>
+  <si>
+    <t>ADC Data 29</t>
+  </si>
+  <si>
+    <t>ADC Data 43</t>
+  </si>
+  <si>
+    <t>ADC Data 1</t>
+  </si>
+  <si>
+    <t>ADC Data 2</t>
+  </si>
+  <si>
+    <t>ADC Data 3</t>
+  </si>
+  <si>
+    <t>ADC Data 4</t>
+  </si>
+  <si>
+    <t>ADC Fault</t>
+  </si>
+  <si>
+    <t>I2C1 Fault</t>
+  </si>
+  <si>
+    <t>I2C1 Master</t>
   </si>
 </sst>
 </file>
@@ -114,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -123,6 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,20 +446,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.08984375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.36328125" customWidth="1"/>
+    <col min="5" max="5" width="22.08984375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -426,117 +470,301 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>16</v>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B17">
         <v>5</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="C17" s="4">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
         <v>6</v>
       </c>
-      <c r="B10">
-        <v>6</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
+      <c r="C18" s="4">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20">
         <v>4</v>
       </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
         <v>5</v>
       </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>15</v>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>